<commit_message>
Mark article as synced
</commit_message>
<xml_diff>
--- a/bestand.xlsx
+++ b/bestand.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>EAN</t>
   </si>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>Creme</t>
-  </si>
-  <si>
-    <t>Last Sync</t>
   </si>
 </sst>
 </file>
@@ -442,7 +439,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="true" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -466,9 +463,6 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
@@ -484,7 +478,7 @@
         <v>8.99</v>
       </c>
       <c r="E2" s="6">
-        <v>45306.751745109956</v>
+        <v>45306.895564331055</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -501,7 +495,7 @@
         <v>2.99</v>
       </c>
       <c r="E3" s="6">
-        <v>45306.75174512209</v>
+        <v>45306.895564331055</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Provide cmd adapter for upload
</commit_message>
<xml_diff>
--- a/bestand.xlsx
+++ b/bestand.xlsx
@@ -478,7 +478,7 @@
         <v>8.99</v>
       </c>
       <c r="E2" s="6">
-        <v>45306.895564331055</v>
+        <v>45307.47846368295</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -495,7 +495,7 @@
         <v>2.99</v>
       </c>
       <c r="E3" s="6">
-        <v>45306.895564331055</v>
+        <v>45307.47846368295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Upload product to otto market api
</commit_message>
<xml_diff>
--- a/bestand.xlsx
+++ b/bestand.xlsx
@@ -478,7 +478,7 @@
         <v>8.99</v>
       </c>
       <c r="E2" s="6">
-        <v>45308.71746227314</v>
+        <v>45313.47044580607</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -495,7 +495,7 @@
         <v>2.99</v>
       </c>
       <c r="E3" s="6">
-        <v>45308.71746227314</v>
+        <v>45313.47044580607</v>
       </c>
     </row>
   </sheetData>

</xml_diff>